<commit_message>
llenar primera parte de la bitacora
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -124,11 +124,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="[$-80A]@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,6 +230,14 @@
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -284,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -304,13 +313,6 @@
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -382,7 +384,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -415,7 +417,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,59 +429,51 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -487,8 +481,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -511,83 +505,87 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,7 +593,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -603,11 +601,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,15 +688,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="T16" activeCellId="0" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="3.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="3.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.88"/>
@@ -847,41 +847,41 @@
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="20"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="26"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
@@ -891,271 +891,272 @@
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="28" t="s">
+      <c r="J10" s="10"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="29" t="s">
+      <c r="M10" s="21"/>
+      <c r="N10" s="27" t="s">
         <v>16</v>
       </c>
       <c r="O10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
     </row>
     <row r="12" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35" t="s">
+      <c r="I12" s="32"/>
+      <c r="J12" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37" t="s">
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="38" t="s">
+      <c r="O12" s="36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="44"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="39"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="37"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="39"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="37"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="39"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="37"/>
+      <c r="T16" s="44"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="39"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="37"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="39"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="37"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="39"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="37"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="39"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="37"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="39"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="37"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="39"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="37"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="39"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="37"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
@@ -1169,12 +1170,12 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="46" t="s">
+      <c r="L24" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="39"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="37"/>
     </row>
     <row r="25" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
@@ -1188,10 +1189,10 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="39"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="37"/>
     </row>
     <row r="26" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
@@ -1228,71 +1229,71 @@
       <c r="O27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="47"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="51"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="50"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="52" t="s">
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="53"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="52"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="53"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="52"/>
     </row>
     <row r="31" customFormat="false" ht="2.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
       <c r="G31" s="1"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="56" t="s">
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
     </row>
     <row r="32" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
@@ -1305,9 +1306,9 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="55"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
@@ -1334,19 +1335,24 @@
       <c r="K34" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="51">
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="J3:O3"/>
     <mergeCell ref="A5:O5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="N7:O7"/>
-    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="J8:K9"/>
     <mergeCell ref="L8:O8"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="L9:O9"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="K11:O11"/>

</xml_diff>